<commit_message>
Ev13CountLimit, Ev14CountLimit, Ev15CountLimit, Ev16CountLimit, Ev17CountLimit 글로벌 상수 추가 및 이벤트명 단일 불필요한 샵프로덕트 아이디 제거, 구매 패키지 이름 제공 등
</commit_message>
<xml_diff>
--- a/Excel/Event.xlsx
+++ b/Excel/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectNameless\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF232D15-D83D-454E-BA01-FEC937F4AD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F777CC2-C6F4-40FC-9F91-4B5068BA901B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1095" windowWidth="24000" windowHeight="11700" xr2:uid="{4309CADF-FF23-49E3-9123-A93F4C6AE535}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4309CADF-FF23-49E3-9123-A93F4C6AE535}"/>
   </bookViews>
   <sheets>
     <sheet name="EventTypeTable" sheetId="1" r:id="rId1"/>
@@ -590,9 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80608E75-A5C0-465B-AF44-ED5B52C77D29}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1196,7 +1194,7 @@
         <v>56</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>86400</v>

</xml_diff>